<commit_message>
added verification on theoretical model (only excel study)
</commit_message>
<xml_diff>
--- a/Analysis/expertiments/hard_game_mode/arrival_boss20_minion10/throughput/experiments_hard_game_mode_throughput.xlsx
+++ b/Analysis/expertiments/hard_game_mode/arrival_boss20_minion10/throughput/experiments_hard_game_mode_throughput.xlsx
@@ -49,70 +49,13 @@
     <t xml:space="preserve">Mean (minion throughput)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Mean (bosses </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">throughput</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Mean (bosses throughput)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Average of means minions </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">throughput</t>
-    </r>
+    <t xml:space="preserve">Average of means minions throughput</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Average of means boss  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">throughput</t>
-    </r>
+    <t xml:space="preserve">Average of means boss  throughput</t>
   </si>
   <si>
     <t xml:space="preserve">minion std deviation</t>
@@ -139,42 +82,10 @@
     <t xml:space="preserve">minion_throughput_stat:vector</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">minion mean </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">throughput</t>
-    </r>
+    <t xml:space="preserve">minion mean throughput</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">boss mean </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">throughput</t>
-    </r>
+    <t xml:space="preserve">boss mean throughput</t>
   </si>
   <si>
     <t xml:space="preserve">minions CI</t>
@@ -211,12 +122,12 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -425,7 +336,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -684,6 +595,67 @@
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$27:$Y$31</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00225627258756764</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00246531589678737</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00248400081979119</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00271101505877585</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00264055994865738</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$27:$Y$31</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00225627258756764</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00246531589678737</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00248400081979119</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00271101505877585</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00264055994865738</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="ff420e"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$U$3:$U$7</c:f>
@@ -789,6 +761,67 @@
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$37:$Y$41</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00230840429323587</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0025703999560382</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00269687568951086</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0028758792475486</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00292367958388698</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$37:$Y$41</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00230840429323587</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0025703999560382</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00269687568951086</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0028758792475486</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00292367958388698</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="ffff00"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$U$3:$U$7</c:f>
@@ -894,6 +927,67 @@
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$47:$Y$51</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00247870989528802</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00261582977434257</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00297186802036459</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00302237061715073</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00289741627646318</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$47:$Y$51</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00247870989528802</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00261582977434257</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00297186802036459</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00302237061715073</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00289741627646318</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="579d1c"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$U$3:$U$7</c:f>
@@ -999,6 +1093,67 @@
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$57:$Y$61</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00260607079686946</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00282017790940763</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00338127627096755</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0033520835721761</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00323484408429151</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$57:$Y$61</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00260607079686946</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00282017790940763</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00338127627096755</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0033520835721761</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00323484408429151</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="7e0021"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$U$3:$U$7</c:f>
@@ -1215,11 +1370,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="46978622"/>
-        <c:axId val="22219885"/>
+        <c:axId val="18741927"/>
+        <c:axId val="130786"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46978622"/>
+        <c:axId val="18741927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,12 +1430,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22219885"/>
+        <c:crossAx val="130786"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="22219885"/>
+        <c:axId val="130786"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.105"/>
@@ -1347,7 +1502,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46978622"/>
+        <c:crossAx val="18741927"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1395,7 +1550,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1654,6 +1809,67 @@
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$32:$Y$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00226234408872217</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00255402166826632</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0026631999689849</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00274667736774658</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00275470347979228</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$32:$Y$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00226234408872217</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00255402166826632</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0026631999689849</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00274667736774658</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00275470347979228</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="ff420e"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$U$3:$U$7</c:f>
@@ -1759,6 +1975,67 @@
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$42:$Y$46</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00238553954349011</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00256866323162304</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00280866866436898</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00278145078339393</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00272093857070618</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$42:$Y$46</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00238553954349011</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00256866323162304</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00280866866436898</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00278145078339393</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00272093857070618</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="ffff00"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$U$3:$U$7</c:f>
@@ -1864,6 +2141,67 @@
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$52:$Y$56</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00253733813582545</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00261446102663466</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00321347265278143</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00318470873148134</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00293831447362596</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$52:$Y$56</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00253733813582545</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00261446102663466</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00321347265278143</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00318470873148134</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00293831447362596</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="579d1c"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$U$3:$U$7</c:f>
@@ -1969,6 +2307,67 @@
             <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$62:$Y$66</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00262680787016781</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00285076184531963</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00342390931978131</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00318260801453719</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00306948937369886</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Y$62:$Y$66</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.00262680787016781</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.00285076184531963</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.00342390931978131</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.00318260801453719</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00306948937369886</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="7e0021"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$U$3:$U$7</c:f>
@@ -2185,11 +2584,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="20628395"/>
-        <c:axId val="1950371"/>
+        <c:axId val="68784227"/>
+        <c:axId val="74200660"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20628395"/>
+        <c:axId val="68784227"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2245,12 +2644,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1950371"/>
+        <c:crossAx val="74200660"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1950371"/>
+        <c:axId val="74200660"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.105"/>
@@ -2317,7 +2716,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20628395"/>
+        <c:crossAx val="68784227"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2365,7 +2764,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2405,10 +2804,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0650229754434508"/>
-          <c:y val="0.137834036568214"/>
-          <c:w val="0.910025198873462"/>
-          <c:h val="0.682489451476793"/>
+          <c:x val="0.0650133386029049"/>
+          <c:y val="0.137846153846154"/>
+          <c:w val="0.909989131508744"/>
+          <c:h val="0.682461538461538"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2531,7 +2930,7 @@
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="000000"/>
+                  <a:srgbClr val="004586"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -2592,11 +2991,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="952644"/>
-        <c:axId val="14931829"/>
+        <c:axId val="75645987"/>
+        <c:axId val="50621036"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="952644"/>
+        <c:axId val="75645987"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2652,12 +3051,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14931829"/>
+        <c:crossAx val="50621036"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14931829"/>
+        <c:axId val="50621036"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.06"/>
@@ -2724,7 +3123,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="952644"/>
+        <c:crossAx val="75645987"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2783,9 +3182,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
-      <xdr:colOff>538920</xdr:colOff>
+      <xdr:colOff>538560</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2793,8 +3192,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="52468920" y="1531440"/>
-        <a:ext cx="12629520" cy="7066440"/>
+        <a:off x="52473960" y="1531440"/>
+        <a:ext cx="12648240" cy="7066080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2813,9 +3212,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>48</xdr:col>
-      <xdr:colOff>55080</xdr:colOff>
+      <xdr:colOff>54720</xdr:colOff>
       <xdr:row>100</xdr:row>
-      <xdr:rowOff>72000</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2823,8 +3222,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="52511760" y="9926640"/>
-        <a:ext cx="12929040" cy="7233840"/>
+        <a:off x="52516800" y="9926640"/>
+        <a:ext cx="12949200" cy="7233480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2843,9 +3242,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>414000</xdr:colOff>
+      <xdr:colOff>413640</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:rowOff>104760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2853,8 +3252,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="44469720" y="6108480"/>
-        <a:ext cx="7285680" cy="4095000"/>
+        <a:off x="44472240" y="6108480"/>
+        <a:ext cx="7286760" cy="4094640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2874,11 +3273,11 @@
   </sheetPr>
   <dimension ref="B1:AD2162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U25" colorId="64" zoomScale="32" zoomScaleNormal="32" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW49" activeCellId="0" sqref="AW49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD37" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BA93" activeCellId="0" sqref="BA93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.19"/>

</xml_diff>